<commit_message>
add JSON data source
</commit_message>
<xml_diff>
--- a/CS/FederationDataSourceExample/OrderHeaders.xlsx
+++ b/CS/FederationDataSourceExample/OrderHeaders.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,48 +20,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t xml:space="preserve">OrderID</t>
   </si>
   <si>
+    <t xml:space="preserve">CustomerID</t>
+  </si>
+  <si>
     <t xml:space="preserve">Status</t>
   </si>
   <si>
     <t xml:space="preserve">Description</t>
   </si>
   <si>
+    <t xml:space="preserve">ANATR</t>
+  </si>
+  <si>
     <t xml:space="preserve">Paid</t>
   </si>
   <si>
     <t xml:space="preserve">Smooth</t>
   </si>
   <si>
+    <t xml:space="preserve">TORTU</t>
+  </si>
+  <si>
     <t xml:space="preserve">Unpaid</t>
   </si>
   <si>
     <t xml:space="preserve">Bright</t>
   </si>
   <si>
+    <t xml:space="preserve">VAFFE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Crisp</t>
   </si>
   <si>
+    <t xml:space="preserve">MEREP</t>
+  </si>
+  <si>
     <t xml:space="preserve">Good</t>
   </si>
   <si>
+    <t xml:space="preserve">PRINI</t>
+  </si>
+  <si>
     <t xml:space="preserve">Excellent</t>
   </si>
   <si>
+    <t xml:space="preserve">HILAA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Poor</t>
   </si>
   <si>
+    <t xml:space="preserve">LEHMS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bad</t>
   </si>
   <si>
+    <t xml:space="preserve">QUEEN</t>
+  </si>
+  <si>
     <t xml:space="preserve">Normal</t>
   </si>
   <si>
+    <t xml:space="preserve">LAMAI</t>
+  </si>
+  <si>
     <t xml:space="preserve">Satisfactory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRANK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WARTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BONAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PERIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUICK</t>
   </si>
 </sst>
 </file>
@@ -72,7 +117,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -103,6 +148,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,12 +199,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -173,17 +229,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -196,170 +252,218 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>10308</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>3</v>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>10319</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>5</v>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>10367</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>3</v>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>10424</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>5</v>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>8</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>10477</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>3</v>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>10490</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>5</v>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>10593</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>3</v>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>10659</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>3</v>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>10923</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>3</v>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>20965</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>3</v>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>21056</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>3</v>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>21698</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>5</v>
+      <c r="B13" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>8</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>21704</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>3</v>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>21917</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>3</v>
+      <c r="B15" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>43901</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>3</v>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>